<commit_message>
back to small ppt
</commit_message>
<xml_diff>
--- a/附件2-谦比希铜矿东南矿体膏体充填智能化精准控制与三维可视化系统建设项目-预算.xlsx
+++ b/附件2-谦比希铜矿东南矿体膏体充填智能化精准控制与三维可视化系统建设项目-预算.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D756EA91-DDD5-EC4A-AE8F-1905A67D907E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FECF084-38C2-1745-BD80-2792D9906B8D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="总预算" sheetId="7" r:id="rId1"/>
-    <sheet name="材料费预算" sheetId="9" r:id="rId2"/>
+    <sheet name="软件开发预算" sheetId="7" r:id="rId1"/>
+    <sheet name="非矿设备配套预算" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
   <si>
     <r>
       <rPr>
@@ -450,509 +450,11 @@
     <t>型号</t>
   </si>
   <si>
-    <t>详细参数</t>
-  </si>
-  <si>
-    <r>
-      <t>阵列卡：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>LSI 9361-8i 2G</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>大容量缓存 支持</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Raid0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>50</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>60</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>IW2200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>准系统（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>C612</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>芯片组双路主板，最大支持</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>内存，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>盘位热插拔，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>500W</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>冗余电源，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>2U</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>机架式）</t>
-    </r>
-  </si>
-  <si>
     <t>网络：双口万兆光纤网卡/含多模光模块</t>
   </si>
   <si>
     <t>总价(元)</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设备材料的购置及运送</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>购置
-及运送费</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>鼠标、键盘、机械硬盘等相关办公用品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>办公用品</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>* 23.8英寸 AH-IPS广视角 127%sRGB广色域 1.5mm窄边框 
-全接口 24 快拆旋转升降支架 电脑显示器</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AOC
-I2490PXZ </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示器</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>软件环境</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>:Ubuntu16.04</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>操作系统</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>资质：认证：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ISO9001</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>国际质量管理体系，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>NVIDIA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>精英级合作伙伴（官网认证），</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>名</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>NVIDIA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>认证工程师；
-服务：厂家工程师三年免费质保服务；三年免费上门，终身软件维护服务。</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>网络：双口千兆网卡（支持网络唤醒，网络冗余，负载均衡等网络高级特性，支持</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>I/O AT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>加速技术），</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>个</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>IPMI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>远程管理口（支持远程开关机、温度监测、调整风扇转速、远程桌面、报错</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="仿宋"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>log</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>收集等）</t>
-    </r>
   </si>
   <si>
     <t>显卡：Nvidia V100
@@ -1106,20 +608,159 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>笔记本电脑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>存储盘：4* 希捷(Seagate)12TB 企业级硬盘
 型号：希捷银河Exos 7E8系列
 接口：SATA接口</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>联想ThinkPad 翼480 英特尔酷睿i7 14英寸轻薄窄边框笔记本电脑（i7-8550U 8G 128GSSD+1T 2G独显 FHD）银</t>
-  </si>
-  <si>
     <t>材料费（系统开发设备、电子耗材、办公用品）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>思腾合力缓存服务器</t>
+  </si>
+  <si>
+    <t>IR2200</t>
+  </si>
+  <si>
+    <t>压力变送器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他电缆等材料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详细参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于实时录入数据、运行大数据平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算服务器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恩菲提供</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU：2* 英特尔 XEON E5-2620V4/8核/16线程/2.1GHz-3.0GHz</t>
+  </si>
+  <si>
+    <t>内存：4* 32GB R-ECC DDR4 2400MHz 服务器内存 支持高级内存纠错、内存镜像</t>
+  </si>
+  <si>
+    <t>系统盘：2* 240G 企业级固态硬盘（Raid1）
+品牌：英特尔     型号：S4510 SSDSC2KB240G801
+性能描述：读560MB/s   写510MB/s</t>
+  </si>
+  <si>
+    <t>缓存盘：2* 2TB PCIE接口 数据中心企业级固态硬盘
+品牌：英特尔     型号：DC P4600 SSDPEDKE020T701
+性能描述：读3290MB/s  写1650MB/s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阵列卡：LSI 9361-8i 2G大容量缓存 支持Raid0、1、5、6、10、50、60</t>
+  </si>
+  <si>
+    <r>
+      <t>IW2200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="仿宋"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>准系统（C612芯片组双路主板，最大支持1T内存，12盘位热插拔，500W冗余电源，2U机架式）</t>
+    </r>
+  </si>
+  <si>
+    <t>网络：双口千兆网卡（支持网络唤醒，网络冗余，负载均衡等网络高级特性，支持I/O AT加速技术），1个IPMI远程管理口（支持远程开关机、温度监测、调整风扇转速、远程桌面、报错log收集等）</t>
+  </si>
+  <si>
+    <t>资质：认证：ISO9001国际质量管理体系，NVIDIA精英级合作伙伴（官网认证），10名NVIDIA认证工程师；
+服务：厂家工程师三年免费质保服务；三年免费上门，终身软件维护服务。</t>
+  </si>
+  <si>
+    <t>软件环境:操作系统根据客户要求安装。</t>
+  </si>
+  <si>
+    <t>软件环境:Ubuntu16.04操作系统</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>井下管道视频智能监控系统</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000万像素，网口，每秒2帧，价格8万，含镜头、光源和保护罩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于监测搅拌机的膏体均匀度，架设在充填站二段搅拌机上方</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">用于监测井下管道压力，安装位置：
+（1）井下680ml
+区域一：钻孔底部，连接4个钻孔的每条管道安装一块压力变送器，用于监测钻孔内部料浆的高度，确定钻孔是否满管，需要4块压力变送器。
+区域二： 680ml-696ml充填钻孔上部水平段2条管路上，每条管路安装个压力变送器，需要2块压力变送器。
+区域三： 680-980ml充填钻孔上部水平段2条管路上安装2个压力变送器。
+（2）井下980 ml
+区域一：钻孔底部，连接2个钻孔的每条管道安装一块压力变送器，用于监测钻孔内部料浆的高度，确定钻孔是否满管，需要2块压力变送器。
+区域二： 980ml中段主进风巷与矿体下盘回/进风道交叉处的水平主管，用于监测980ml两个充填主管压力，需要2块压力变送器。
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于井下管道监控
+安装位置：
+（1）井下680 ml，设1个监测点，监测地表至680ml钻孔底部管道实时状态，需要1个摄像头。
+（2）680ml水平管道，设置2个监测点，一个监测北采区方向，一个监测南采区方向，每个监测点2个摄像头，共需4个摄像头。
+（3）井下696ml，设1个监测点，监测680ml-696ml钻孔底部管道实时状态，需要1个摄像头。
+（4）井下980 ml，设1个监测点，监测680ml-980ml钻孔底部管道实时状态，需要1个摄像头。
+（5）井下980 m水平管道，设置1个监测点，设置2个摄像头。
+（6）充填站两台二段搅拌机上方，各1个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿井摄像头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通摄像头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GEV-B6620M-TF097 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nikon Rayfact IL 40mm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1130,7 +771,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,39 +907,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="9"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="仿宋"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="仿宋"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="仿宋"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -1306,16 +914,81 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="微软雅黑"/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color indexed="8"/>
+      <name val="仿宋"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="16"/>
-      <name val="微软雅黑"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color indexed="9"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color indexed="9"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color indexed="8"/>
+      <name val="仿宋"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="仿宋"/>
+      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1350,7 +1023,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1509,253 +1182,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="1">
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal style="medium">
-        <color indexed="8"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1859,68 +1296,55 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="26" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="5" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2069,42 +1493,25 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2445,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -2469,30 +1876,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="51" customHeight="1">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="32.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2505,25 +1912,25 @@
       <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="58"/>
     </row>
     <row r="3" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="59"/>
+      <c r="E3" s="56"/>
       <c r="F3" s="13"/>
       <c r="G3" s="14">
         <v>4</v>
@@ -2535,22 +1942,22 @@
         <f>G3*H3</f>
         <v>4</v>
       </c>
-      <c r="J3" s="70">
+      <c r="J3" s="67">
         <f>SUM(I3:I5)</f>
         <v>19.5</v>
       </c>
-      <c r="K3" s="71"/>
+      <c r="K3" s="68"/>
     </row>
     <row r="4" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A4" s="67"/>
-      <c r="B4" s="66"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="12">
         <v>2</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="59"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="13"/>
       <c r="G4" s="29">
         <v>5</v>
@@ -2559,22 +1966,22 @@
         <v>1.5</v>
       </c>
       <c r="I4" s="33">
-        <f t="shared" ref="I4:I26" si="0">G4*H4</f>
+        <f t="shared" ref="I4:I27" si="0">G4*H4</f>
         <v>7.5</v>
       </c>
-      <c r="J4" s="72"/>
-      <c r="K4" s="73"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A5" s="67"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="12">
         <v>3</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="57"/>
       <c r="F5" s="13"/>
       <c r="G5" s="14">
         <v>4</v>
@@ -2586,23 +1993,23 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="72"/>
     </row>
     <row r="6" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="62" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="60"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="13"/>
       <c r="G6" s="14">
         <v>3</v>
@@ -2614,22 +2021,22 @@
         <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
-      <c r="J6" s="70">
+      <c r="J6" s="67">
         <f>SUM(I6:I9)</f>
         <v>26.4</v>
       </c>
-      <c r="K6" s="71"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A7" s="69"/>
-      <c r="B7" s="65"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="57"/>
       <c r="F7" s="13"/>
       <c r="G7" s="14">
         <v>5</v>
@@ -2641,19 +2048,19 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="73"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A8" s="69"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="12">
         <v>3</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="60"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="13"/>
       <c r="G8" s="33">
         <v>5</v>
@@ -2665,19 +2072,19 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="73"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="70"/>
     </row>
     <row r="9" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A9" s="69"/>
-      <c r="B9" s="65"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="12">
         <v>4</v>
       </c>
-      <c r="D9" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="60"/>
+      <c r="D9" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="57"/>
       <c r="F9" s="13"/>
       <c r="G9" s="14">
         <v>5</v>
@@ -2689,24 +2096,24 @@
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="75"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="72"/>
     </row>
     <row r="10" spans="1:11" s="20" customFormat="1" ht="18" customHeight="1">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="98" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="16">
         <v>1</v>
       </c>
-      <c r="D10" s="84" t="s">
-        <v>59</v>
+      <c r="D10" s="81" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19">
@@ -2719,24 +2126,24 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="J10" s="104">
+      <c r="J10" s="101">
         <f>SUM(I10:I16)</f>
         <v>64.800000000000011</v>
       </c>
-      <c r="K10" s="77">
-        <f>SUM(J10:J26)</f>
+      <c r="K10" s="74">
+        <f>SUM(J10:J27)</f>
         <v>132.95000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A11" s="83"/>
-      <c r="B11" s="102"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="16">
         <v>2</v>
       </c>
-      <c r="D11" s="83"/>
+      <c r="D11" s="80"/>
       <c r="E11" s="17" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="19">
@@ -2749,18 +2156,18 @@
         <f t="shared" si="0"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="J11" s="96"/>
-      <c r="K11" s="79"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A12" s="83"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="16">
         <v>3</v>
       </c>
-      <c r="D12" s="83"/>
+      <c r="D12" s="80"/>
       <c r="E12" s="17" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19">
@@ -2773,18 +2180,18 @@
         <f t="shared" si="0"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="J12" s="96"/>
-      <c r="K12" s="79"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="76"/>
     </row>
     <row r="13" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A13" s="83"/>
-      <c r="B13" s="102"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="16">
         <v>4</v>
       </c>
-      <c r="D13" s="83"/>
+      <c r="D13" s="80"/>
       <c r="E13" s="30" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F13" s="31"/>
       <c r="G13" s="31">
@@ -2797,18 +2204,18 @@
         <f t="shared" si="0"/>
         <v>4.8000000000000007</v>
       </c>
-      <c r="J13" s="96"/>
-      <c r="K13" s="79"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="76"/>
     </row>
     <row r="14" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A14" s="83"/>
-      <c r="B14" s="102"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="99"/>
       <c r="C14" s="16">
         <v>5</v>
       </c>
-      <c r="D14" s="83"/>
+      <c r="D14" s="80"/>
       <c r="E14" s="30" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="31">
@@ -2821,18 +2228,18 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="J14" s="96"/>
-      <c r="K14" s="79"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="76"/>
     </row>
     <row r="15" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A15" s="83"/>
-      <c r="B15" s="102"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="16">
         <v>6</v>
       </c>
-      <c r="D15" s="83"/>
+      <c r="D15" s="80"/>
       <c r="E15" s="21" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="19">
@@ -2845,16 +2252,16 @@
         <f t="shared" si="0"/>
         <v>6.4</v>
       </c>
-      <c r="J15" s="96"/>
-      <c r="K15" s="79"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="76"/>
     </row>
     <row r="16" spans="1:11" s="20" customFormat="1" ht="18">
-      <c r="A16" s="83"/>
-      <c r="B16" s="102"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="16">
         <v>7</v>
       </c>
-      <c r="D16" s="85"/>
+      <c r="D16" s="82"/>
       <c r="E16" s="21" t="s">
         <v>14</v>
       </c>
@@ -2869,20 +2276,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J16" s="97"/>
-      <c r="K16" s="79"/>
+      <c r="J16" s="94"/>
+      <c r="K16" s="76"/>
     </row>
     <row r="17" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A17" s="83"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="16">
         <v>8</v>
       </c>
-      <c r="D17" s="84" t="s">
-        <v>62</v>
+      <c r="D17" s="81" t="s">
+        <v>49</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="19">
@@ -2895,223 +2302,223 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J17" s="104">
-        <f>SUM(I17:I19)</f>
+      <c r="J17" s="101">
+        <f>SUM(I17:I20)</f>
         <v>36</v>
       </c>
-      <c r="K17" s="79"/>
+      <c r="K17" s="76"/>
     </row>
     <row r="18" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A18" s="83"/>
-      <c r="B18" s="102"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="99"/>
       <c r="C18" s="16">
         <v>9</v>
       </c>
-      <c r="D18" s="83"/>
+      <c r="D18" s="80"/>
       <c r="E18" s="21" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H18" s="32">
         <v>2</v>
       </c>
       <c r="I18" s="33">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="J18" s="96"/>
-      <c r="K18" s="79"/>
+        <v>8</v>
+      </c>
+      <c r="J18" s="93"/>
+      <c r="K18" s="76"/>
     </row>
     <row r="19" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A19" s="83"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="16">
         <v>10</v>
       </c>
-      <c r="D19" s="83"/>
+      <c r="D19" s="80"/>
       <c r="E19" s="21" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F19" s="18"/>
-      <c r="G19" s="32">
+      <c r="G19" s="36">
+        <v>4</v>
+      </c>
+      <c r="H19" s="36">
+        <v>2</v>
+      </c>
+      <c r="I19" s="35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J19" s="93"/>
+      <c r="K19" s="76"/>
+    </row>
+    <row r="20" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A20" s="80"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="16">
+        <v>11</v>
+      </c>
+      <c r="D20" s="80"/>
+      <c r="E20" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="32">
+        <v>4</v>
+      </c>
+      <c r="H20" s="32">
+        <v>2</v>
+      </c>
+      <c r="I20" s="33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J20" s="94"/>
+      <c r="K20" s="76"/>
+    </row>
+    <row r="21" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A21" s="34"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="16">
+        <v>12</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="32">
         <v>6</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H21" s="32">
         <v>2</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I21" s="33">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J19" s="97"/>
-      <c r="K19" s="79"/>
-    </row>
-    <row r="20" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A20" s="34"/>
-      <c r="B20" s="102"/>
-      <c r="C20" s="16">
-        <v>11</v>
-      </c>
-      <c r="D20" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="18"/>
-      <c r="G20" s="32">
-        <v>6</v>
-      </c>
-      <c r="H20" s="32">
+      <c r="J21" s="95">
+        <f>SUM(I21:I24)</f>
+        <v>28.4</v>
+      </c>
+      <c r="K21" s="76"/>
+    </row>
+    <row r="22" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A22" s="34"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="16">
+        <v>13</v>
+      </c>
+      <c r="D22" s="80"/>
+      <c r="E22" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" s="32">
         <v>2</v>
       </c>
-      <c r="I20" s="33">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="J20" s="98">
-        <f>SUM(I20:I23)</f>
-        <v>28.4</v>
-      </c>
-      <c r="K20" s="79"/>
-    </row>
-    <row r="21" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A21" s="34"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="16">
-        <v>12</v>
-      </c>
-      <c r="D21" s="83"/>
-      <c r="E21" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="32">
-        <v>2</v>
-      </c>
-      <c r="H21" s="32">
+      <c r="H22" s="32">
         <v>1.6</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I22" s="33">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="J21" s="98"/>
-      <c r="K21" s="79"/>
-    </row>
-    <row r="22" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A22" s="34"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="16">
-        <v>13</v>
-      </c>
-      <c r="D22" s="83"/>
-      <c r="E22" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="32">
+      <c r="J22" s="95"/>
+      <c r="K22" s="76"/>
+    </row>
+    <row r="23" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A23" s="34"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="16">
+        <v>14</v>
+      </c>
+      <c r="D23" s="80"/>
+      <c r="E23" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" s="32">
         <v>5</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H23" s="32">
         <v>2</v>
       </c>
-      <c r="I22" s="33">
+      <c r="I23" s="33">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="J22" s="98"/>
-      <c r="K22" s="79"/>
-    </row>
-    <row r="23" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A23" s="34"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="16">
-        <v>14</v>
-      </c>
-      <c r="D23" s="85"/>
-      <c r="E23" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="32">
+      <c r="J23" s="95"/>
+      <c r="K23" s="76"/>
+    </row>
+    <row r="24" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A24" s="34"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="16">
+        <v>15</v>
+      </c>
+      <c r="D24" s="82"/>
+      <c r="E24" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="32">
         <v>2</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H24" s="32">
         <v>1.6</v>
       </c>
-      <c r="I23" s="33">
+      <c r="I24" s="33">
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-      <c r="J23" s="98"/>
-      <c r="K23" s="79"/>
-    </row>
-    <row r="24" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A24" s="34"/>
-      <c r="B24" s="102"/>
-      <c r="C24" s="16">
-        <v>15</v>
-      </c>
-      <c r="D24" s="84" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="32">
+      <c r="J24" s="95"/>
+      <c r="K24" s="76"/>
+    </row>
+    <row r="25" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A25" s="34"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="16">
+        <v>16</v>
+      </c>
+      <c r="D25" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="32">
         <v>1.5</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H25" s="32">
         <v>1.5</v>
       </c>
-      <c r="I24" s="33">
+      <c r="I25" s="33">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="J24" s="104">
-        <f>SUM(I24:I26)</f>
+      <c r="J25" s="101">
+        <f>SUM(I25:I27)</f>
         <v>3.75</v>
       </c>
-      <c r="K24" s="79"/>
-    </row>
-    <row r="25" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A25" s="34"/>
-      <c r="B25" s="102"/>
-      <c r="C25" s="16">
-        <v>16</v>
-      </c>
-      <c r="D25" s="83"/>
-      <c r="E25" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="18"/>
-      <c r="G25" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="H25" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="I25" s="33">
-        <f t="shared" si="0"/>
-        <v>0.75</v>
-      </c>
-      <c r="J25" s="96"/>
-      <c r="K25" s="79"/>
+      <c r="K25" s="76"/>
     </row>
     <row r="26" spans="1:14" s="20" customFormat="1" ht="18">
       <c r="A26" s="34"/>
-      <c r="B26" s="103"/>
+      <c r="B26" s="99"/>
       <c r="C26" s="16">
         <v>17</v>
       </c>
-      <c r="D26" s="85"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="21" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="32">
@@ -3124,201 +2531,217 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J26" s="97"/>
-      <c r="K26" s="81"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="76"/>
     </row>
     <row r="27" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="34"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="16">
+        <v>18</v>
+      </c>
+      <c r="D27" s="82"/>
+      <c r="E27" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="I27" s="33">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="J27" s="94"/>
+      <c r="K27" s="78"/>
+    </row>
+    <row r="28" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A28" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B28" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C28" s="22">
         <v>1</v>
       </c>
-      <c r="D27" s="82" t="s">
+      <c r="D28" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="82"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24">
+      <c r="E28" s="79"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24">
         <v>3</v>
-      </c>
-      <c r="H27" s="24">
-        <v>1</v>
-      </c>
-      <c r="I27" s="29">
-        <f t="shared" ref="I27" si="1">G27*H27</f>
-        <v>3</v>
-      </c>
-      <c r="J27" s="82">
-        <f>SUM(I27:I28)</f>
-        <v>9</v>
-      </c>
-      <c r="K27" s="82"/>
-    </row>
-    <row r="28" spans="1:14" s="20" customFormat="1" ht="77.5" customHeight="1">
-      <c r="A28" s="92"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="22">
-        <v>2</v>
-      </c>
-      <c r="D28" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="82"/>
-      <c r="F28" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="24">
-        <v>6</v>
       </c>
       <c r="H28" s="24">
         <v>1</v>
       </c>
-      <c r="I28" s="24">
-        <f>G28*H28</f>
+      <c r="I28" s="29">
+        <f t="shared" ref="I28" si="1">G28*H28</f>
+        <v>3</v>
+      </c>
+      <c r="J28" s="79">
+        <f>SUM(I28:I29)</f>
+        <v>9</v>
+      </c>
+      <c r="K28" s="79"/>
+    </row>
+    <row r="29" spans="1:14" s="20" customFormat="1" ht="77.5" customHeight="1">
+      <c r="A29" s="89"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="22">
+        <v>2</v>
+      </c>
+      <c r="D29" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="79"/>
+      <c r="F29" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="24">
         <v>6</v>
       </c>
-      <c r="J28" s="82"/>
-      <c r="K28" s="82"/>
-      <c r="N28" s="20">
-        <f>SUM(J3,J6,K10,J27,I30,I31,I32)</f>
+      <c r="H29" s="24">
+        <v>1</v>
+      </c>
+      <c r="I29" s="24">
+        <f>G29*H29</f>
+        <v>6</v>
+      </c>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="N29" s="20">
+        <f>SUM(J3,J6,K10,J28,I31,I32,I33)</f>
         <v>240.95000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="20" customFormat="1" ht="37">
-      <c r="A29" s="84" t="s">
+    <row r="30" spans="1:14" s="20" customFormat="1" ht="37">
+      <c r="A30" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="93" t="s">
+      <c r="B30" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="16">
+      <c r="C30" s="16">
         <v>1</v>
       </c>
-      <c r="D29" s="98" t="s">
+      <c r="D30" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="E29" s="98"/>
-      <c r="F29" s="27" t="s">
+      <c r="E30" s="95"/>
+      <c r="F30" s="27" t="s">
         <v>30</v>
-      </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19">
-        <f>N28*0.149425</f>
-        <v>36.003953750000001</v>
-      </c>
-      <c r="J29" s="76">
-        <f>SUM(I29:I32)</f>
-        <v>89.103953750000002</v>
-      </c>
-      <c r="K29" s="77"/>
-    </row>
-    <row r="30" spans="1:14" s="20" customFormat="1" ht="55">
-      <c r="A30" s="96"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="16">
-        <v>2</v>
-      </c>
-      <c r="D30" s="98" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="98"/>
-      <c r="F30" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19">
+        <f>N29*0.149425</f>
+        <v>36.003953750000001</v>
+      </c>
+      <c r="J30" s="73">
+        <f>SUM(I30:I33)</f>
+        <v>89.103953750000002</v>
+      </c>
+      <c r="K30" s="74"/>
+    </row>
+    <row r="31" spans="1:14" s="20" customFormat="1" ht="55">
+      <c r="A31" s="93"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="16">
+        <v>2</v>
+      </c>
+      <c r="D31" s="95" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="95"/>
+      <c r="F31" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19">
         <v>13</v>
       </c>
-      <c r="J30" s="78"/>
-      <c r="K30" s="79"/>
-    </row>
-    <row r="31" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A31" s="96"/>
-      <c r="B31" s="94"/>
-      <c r="C31" s="16">
+      <c r="J31" s="75"/>
+      <c r="K31" s="76"/>
+    </row>
+    <row r="32" spans="1:14" s="20" customFormat="1" ht="18">
+      <c r="A32" s="93"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="16">
         <v>3</v>
       </c>
-      <c r="D31" s="99" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="100"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28">
+      <c r="D32" s="96" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="97"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28">
         <v>15.1</v>
       </c>
-      <c r="J31" s="78"/>
-      <c r="K31" s="79"/>
-    </row>
-    <row r="32" spans="1:14" s="20" customFormat="1" ht="18">
-      <c r="A32" s="97"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="16">
+      <c r="J32" s="75"/>
+      <c r="K32" s="76"/>
+    </row>
+    <row r="33" spans="1:11" s="20" customFormat="1" ht="18">
+      <c r="A33" s="94"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="16">
         <v>4</v>
       </c>
-      <c r="D32" s="98" t="s">
+      <c r="D33" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="98"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19">
+      <c r="E33" s="95"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="19">
         <v>25</v>
       </c>
-      <c r="H32" s="19">
+      <c r="H33" s="19">
         <v>1</v>
       </c>
-      <c r="I32" s="19">
-        <f>G32*H32</f>
+      <c r="I33" s="19">
+        <f>G33*H33</f>
         <v>25</v>
       </c>
-      <c r="J32" s="80"/>
-      <c r="K32" s="81"/>
-    </row>
-    <row r="33" spans="1:11" s="15" customFormat="1" ht="18">
-      <c r="A33" s="86" t="s">
+      <c r="J33" s="77"/>
+      <c r="K33" s="78"/>
+    </row>
+    <row r="34" spans="1:11" s="15" customFormat="1" ht="18">
+      <c r="A34" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="87"/>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="88"/>
-      <c r="J33" s="69">
-        <f>SUM(N28,J29)</f>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="66">
+        <f>SUM(N29,J30)</f>
         <v>330.05395375000001</v>
       </c>
-      <c r="K33" s="69"/>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1">
+      <c r="K34" s="66"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
+      <c r="F35" s="4"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
+      <c r="K35" s="4"/>
     </row>
     <row r="36" spans="1:11" s="4" customFormat="1">
       <c r="D36" s="9"/>
@@ -3328,31 +2751,29 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="38" spans="1:11">
-      <c r="F38" s="4"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="J38" s="1"/>
+    <row r="37" spans="1:11" s="4" customFormat="1">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="39" spans="1:11">
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:11">
       <c r="F40" s="4"/>
-      <c r="G40" s="7"/>
+      <c r="G40" s="5"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
       <c r="F41" s="4"/>
       <c r="G41" s="7"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="4"/>
     </row>
     <row r="42" spans="1:11">
       <c r="D42" s="11"/>
@@ -3362,6 +2783,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
+      <c r="K42" s="4"/>
     </row>
     <row r="43" spans="1:11">
       <c r="D43" s="11"/>
@@ -3466,38 +2888,47 @@
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="5"/>
+      <c r="G54" s="7"/>
       <c r="H54" s="5"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
+    <row r="55" spans="4:10">
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="K10:K26"/>
-    <mergeCell ref="B10:B26"/>
-    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="K10:K27"/>
+    <mergeCell ref="B10:B27"/>
+    <mergeCell ref="D25:D27"/>
     <mergeCell ref="J10:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J26"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="J17:J20"/>
+    <mergeCell ref="J21:J24"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="A10:A20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
     <mergeCell ref="D10:D16"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="J30:K33"/>
+    <mergeCell ref="J28:K29"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="J29:K32"/>
-    <mergeCell ref="J27:K28"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D5:E5"/>
@@ -3522,220 +2953,407 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656BFDB5-BAC8-4BB0-8CB4-B3D4455992F3}">
-  <dimension ref="A1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0860B3-CE02-D248-9ED4-DD089F3B5290}">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:K1"/>
+    <sheetView topLeftCell="A21" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="11" style="35" customWidth="1"/>
-    <col min="3" max="3" width="57.1640625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="35" customWidth="1"/>
-    <col min="5" max="254" width="9" style="35" customWidth="1"/>
-    <col min="255" max="255" width="9" style="35" bestFit="1" customWidth="1"/>
-    <col min="256" max="16384" width="7.83203125" style="35"/>
+    <col min="1" max="2" width="26.33203125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="42.5" style="38" customWidth="1"/>
+    <col min="4" max="4" width="97.83203125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="97.83203125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="49" customFormat="1" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" ht="54">
+      <c r="A1" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="33" customHeight="1">
+      <c r="A2" s="103" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="103">
+        <v>1</v>
+      </c>
+      <c r="C2" s="103" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="102">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="35" customHeight="1">
+      <c r="A3" s="103"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="103"/>
+      <c r="F3" s="102"/>
+    </row>
+    <row r="4" spans="1:6" ht="68" customHeight="1">
+      <c r="A4" s="103"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="103"/>
+      <c r="F4" s="102"/>
+    </row>
+    <row r="5" spans="1:6" ht="60">
+      <c r="A5" s="103"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="103"/>
+      <c r="F5" s="102"/>
+    </row>
+    <row r="6" spans="1:6" ht="39" customHeight="1">
+      <c r="A6" s="103"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="103"/>
+      <c r="F6" s="102"/>
+    </row>
+    <row r="7" spans="1:6" ht="46" customHeight="1">
+      <c r="A7" s="103"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="103"/>
+      <c r="F7" s="102"/>
+    </row>
+    <row r="8" spans="1:6" ht="37" customHeight="1">
+      <c r="A8" s="103"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-    </row>
-    <row r="2" spans="1:11" ht="46.25" customHeight="1">
-      <c r="A2" s="108" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="111" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="114">
+      <c r="E8" s="103"/>
+      <c r="F8" s="102"/>
+    </row>
+    <row r="9" spans="1:6" ht="71" customHeight="1">
+      <c r="A9" s="103"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="103"/>
+      <c r="F9" s="102"/>
+    </row>
+    <row r="10" spans="1:6" ht="76" customHeight="1">
+      <c r="A10" s="103"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
+      <c r="D10" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="103"/>
+      <c r="F10" s="102"/>
+    </row>
+    <row r="11" spans="1:6" ht="37" customHeight="1">
+      <c r="A11" s="103"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="103"/>
+      <c r="F11" s="102"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="A12" s="104" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="104">
+        <v>1</v>
+      </c>
+      <c r="C12" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="104">
         <v>136000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="49.25" customHeight="1">
-      <c r="A3" s="109"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="115"/>
-    </row>
-    <row r="4" spans="1:11" ht="54.5" customHeight="1">
-      <c r="A4" s="109"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="115"/>
-    </row>
-    <row r="5" spans="1:11" ht="54" customHeight="1">
-      <c r="A5" s="109"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="115"/>
-    </row>
-    <row r="6" spans="1:11" ht="36" customHeight="1">
-      <c r="A6" s="109"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="115"/>
-    </row>
-    <row r="7" spans="1:11" ht="48">
-      <c r="A7" s="109"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="115"/>
-    </row>
-    <row r="8" spans="1:11" ht="45.5" customHeight="1">
-      <c r="A8" s="109"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="46" t="s">
+    <row r="13" spans="1:6" ht="20">
+      <c r="A13" s="104"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+    </row>
+    <row r="14" spans="1:6" ht="60">
+      <c r="A14" s="104"/>
+      <c r="B14" s="104"/>
+      <c r="C14" s="105"/>
+      <c r="D14" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="104"/>
+      <c r="F14" s="104"/>
+    </row>
+    <row r="15" spans="1:6" ht="60">
+      <c r="A15" s="104"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="104"/>
+      <c r="F15" s="104"/>
+    </row>
+    <row r="16" spans="1:6" ht="40">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+    </row>
+    <row r="17" spans="1:6" ht="60">
+      <c r="A17" s="104"/>
+      <c r="B17" s="104"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="104"/>
+      <c r="F17" s="104"/>
+    </row>
+    <row r="18" spans="1:6" ht="20">
+      <c r="A18" s="104"/>
+      <c r="B18" s="104"/>
+      <c r="C18" s="105"/>
+      <c r="D18" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
+    </row>
+    <row r="19" spans="1:6" ht="40">
+      <c r="A19" s="104"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+    </row>
+    <row r="20" spans="1:6" ht="20">
+      <c r="A20" s="104"/>
+      <c r="B20" s="104"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="104"/>
+      <c r="F20" s="104"/>
+    </row>
+    <row r="21" spans="1:6" ht="60">
+      <c r="A21" s="104"/>
+      <c r="B21" s="104"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+    </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E22" s="104"/>
+      <c r="F22" s="104"/>
+    </row>
+    <row r="23" spans="1:6" ht="20">
+      <c r="A23" s="104"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="104"/>
+      <c r="F23" s="104"/>
+    </row>
+    <row r="24" spans="1:6" ht="27">
+      <c r="A24" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="51">
+        <v>2</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="108"/>
+      <c r="E24" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="51">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="324">
+      <c r="A25" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="51">
+        <v>9</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="51">
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="81" customHeight="1">
+      <c r="A26" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="51">
+        <v>5</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="409" customHeight="1">
+      <c r="A27" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="51">
+        <v>12</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="E27" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="51">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="115"/>
-    </row>
-    <row r="9" spans="1:11" ht="49.25" customHeight="1">
-      <c r="A9" s="109"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="115"/>
-    </row>
-    <row r="10" spans="1:11" ht="31.25" customHeight="1">
-      <c r="A10" s="109"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="115"/>
-    </row>
-    <row r="11" spans="1:11" ht="73.75" customHeight="1">
-      <c r="A11" s="109"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="115"/>
-    </row>
-    <row r="12" spans="1:11" ht="69" customHeight="1">
-      <c r="A12" s="109"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="115"/>
-    </row>
-    <row r="13" spans="1:11" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="110"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="116"/>
-    </row>
-    <row r="14" spans="1:11" ht="36" customHeight="1" thickBot="1">
-      <c r="A14" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="55">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="46.75" customHeight="1" thickBot="1">
-      <c r="A15" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="37">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="46.75" customHeight="1" thickBot="1">
-      <c r="A16" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="37">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="46.75" customHeight="1" thickBot="1">
-      <c r="A17" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="37">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="40.25" customHeight="1" thickBot="1">
-      <c r="A18" s="105" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="106"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="36">
-        <f>SUM(D17,D16,D15,D14,D2)</f>
-        <v>151000</v>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="52">
+        <f>SUM(F2:F29)</f>
+        <v>1248000</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="5">
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="D2:D13"/>
+  <mergeCells count="11">
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="C2:C11"/>
+    <mergeCell ref="F2:F11"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="A12:A23"/>
+    <mergeCell ref="B12:B23"/>
+    <mergeCell ref="C12:C23"/>
+    <mergeCell ref="F12:F23"/>
+    <mergeCell ref="E2:E11"/>
+    <mergeCell ref="E12:E23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>